<commit_message>
update swap control signals in the excel file
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Workspaces\3rd-Year\Architecture\Pipelined-Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16672578-99FE-41FD-85C2-4F8728AE7AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF93C7B-1B6C-4B7E-968E-F00AC3870C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1785" windowWidth="9615" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -357,9 +357,6 @@
     <t>1011</t>
   </si>
   <si>
-    <t>0000100x000110101011xx1</t>
-  </si>
-  <si>
     <t>0101100x001110001011xx1</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>0000000x0001000010xxxx0</t>
+  </si>
+  <si>
+    <t>0000100x000110101011xx0</t>
   </si>
 </sst>
 </file>
@@ -790,9 +790,9 @@
   </sheetPr>
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -928,18 +928,18 @@
         <v>16</v>
       </c>
       <c r="T2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="4" t="str">
         <f>CONCATENATE(C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2)</f>
-        <v>0000100x000110101011xx1</v>
+        <v>0000100x000110101011xx0</v>
       </c>
       <c r="V2" s="4"/>
       <c r="W2" s="4">
         <v>10001</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1012,7 +1012,7 @@
         <v>10101</v>
       </c>
       <c r="X3" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1085,7 +1085,7 @@
         <v>10110</v>
       </c>
       <c r="X4" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1158,7 +1158,7 @@
         <v>10111</v>
       </c>
       <c r="X5" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1231,7 +1231,7 @@
         <v>11000</v>
       </c>
       <c r="X6" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1304,7 +1304,7 @@
         <v>10010</v>
       </c>
       <c r="X7" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1377,7 +1377,7 @@
         <v>10011</v>
       </c>
       <c r="X8" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1450,7 +1450,7 @@
         <v>10100</v>
       </c>
       <c r="X9" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1523,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="X10" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1596,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="X11" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -1669,7 +1669,7 @@
         <v>11010</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y12" s="5"/>
     </row>
@@ -1743,7 +1743,7 @@
         <v>89</v>
       </c>
       <c r="X13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -1816,7 +1816,7 @@
         <v>101</v>
       </c>
       <c r="X14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>91</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y15" s="5"/>
     </row>
@@ -1963,7 +1963,7 @@
         <v>92</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y16" s="5"/>
     </row>
@@ -2037,7 +2037,7 @@
         <v>93</v>
       </c>
       <c r="X17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
@@ -2110,7 +2110,7 @@
         <v>94</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y18" s="5"/>
     </row>
@@ -2184,7 +2184,7 @@
         <v>95</v>
       </c>
       <c r="X19" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Y19" s="5"/>
     </row>
@@ -2258,7 +2258,7 @@
         <v>96</v>
       </c>
       <c r="X20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
@@ -2331,7 +2331,7 @@
         <v>97</v>
       </c>
       <c r="X21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
@@ -2404,7 +2404,7 @@
         <v>98</v>
       </c>
       <c r="X22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -2477,7 +2477,7 @@
         <v>99</v>
       </c>
       <c r="X23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -2550,7 +2550,7 @@
         <v>100</v>
       </c>
       <c r="X24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -2623,7 +2623,7 @@
         <v>101</v>
       </c>
       <c r="X25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -2696,7 +2696,7 @@
         <v>102</v>
       </c>
       <c r="X26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
@@ -2769,7 +2769,7 @@
         <v>103</v>
       </c>
       <c r="X27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -2842,7 +2842,7 @@
         <v>104</v>
       </c>
       <c r="X28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -2915,7 +2915,7 @@
         <v>105</v>
       </c>
       <c r="X29" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Y29" s="5"/>
     </row>

</xml_diff>

<commit_message>
fix IADD alu opcode in control unit
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Workspaces\3rd-Year\Architecture\Pipelined-Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF93C7B-1B6C-4B7E-968E-F00AC3870C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D25154-7232-4A70-A86F-8F9AA7BFD60D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="134">
   <si>
     <t>operation</t>
   </si>
@@ -240,9 +240,6 @@
     <t>0111</t>
   </si>
   <si>
-    <t>1010</t>
-  </si>
-  <si>
     <t>00</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>000001000001000010xxxx0</t>
   </si>
   <si>
-    <t>1010100x001100001001x0x</t>
-  </si>
-  <si>
     <t>0000001110000100xx000xx</t>
   </si>
   <si>
@@ -433,6 +427,9 @@
   </si>
   <si>
     <t>0000100x000110101011xx0</t>
+  </si>
+  <si>
+    <t>0101100x001100001001x0x</t>
   </si>
 </sst>
 </file>
@@ -791,8 +788,8 @@
   <dimension ref="A1:Y71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X2" sqref="X2"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -805,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -820,16 +817,16 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -864,7 +861,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
@@ -874,7 +871,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>63</v>
@@ -939,7 +936,7 @@
         <v>10001</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -947,7 +944,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>67</v>
@@ -1012,7 +1009,7 @@
         <v>10101</v>
       </c>
       <c r="X3" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1020,7 +1017,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>68</v>
@@ -1085,7 +1082,7 @@
         <v>10110</v>
       </c>
       <c r="X4" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1093,7 +1090,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>69</v>
@@ -1158,7 +1155,7 @@
         <v>10111</v>
       </c>
       <c r="X5" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1166,7 +1163,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="13">
         <v>1000</v>
@@ -1231,7 +1228,7 @@
         <v>11000</v>
       </c>
       <c r="X6" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1239,7 +1236,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>64</v>
@@ -1284,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R7" s="26" t="s">
         <v>16</v>
@@ -1304,7 +1301,7 @@
         <v>10010</v>
       </c>
       <c r="X7" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1312,7 +1309,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>65</v>
@@ -1357,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R8" s="26" t="s">
         <v>16</v>
@@ -1377,7 +1374,7 @@
         <v>10011</v>
       </c>
       <c r="X8" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1385,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>66</v>
@@ -1430,7 +1427,7 @@
         <v>10</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R9" s="26" t="s">
         <v>16</v>
@@ -1450,7 +1447,7 @@
         <v>10100</v>
       </c>
       <c r="X9" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1458,7 +1455,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="17">
         <v>1001</v>
@@ -1503,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R10" s="26" t="s">
         <v>16</v>
@@ -1523,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="X10" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1531,7 +1528,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="17">
         <v>1010</v>
@@ -1576,7 +1573,7 @@
         <v>10</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R11" s="26" t="s">
         <v>16</v>
@@ -1596,7 +1593,7 @@
         <v>10</v>
       </c>
       <c r="X11" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -1604,7 +1601,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>63</v>
@@ -1646,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="P12" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R12" s="32" t="s">
         <v>16</v>
@@ -1669,7 +1666,7 @@
         <v>11010</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y12" s="5"/>
     </row>
@@ -1678,7 +1675,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>63</v>
@@ -1720,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="20">
         <v>10</v>
@@ -1740,10 +1737,10 @@
       </c>
       <c r="V13" s="4"/>
       <c r="W13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="X13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -1751,10 +1748,10 @@
         <v>33</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1793,10 +1790,10 @@
         <v>0</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R14" s="19" t="s">
         <v>16</v>
@@ -1816,7 +1813,7 @@
         <v>101</v>
       </c>
       <c r="X14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -1824,7 +1821,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>63</v>
@@ -1866,10 +1863,10 @@
         <v>0</v>
       </c>
       <c r="P15" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q15" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R15" s="32">
         <v>0</v>
@@ -1886,10 +1883,10 @@
       </c>
       <c r="V15" s="33"/>
       <c r="W15" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y15" s="5"/>
     </row>
@@ -1898,7 +1895,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>63</v>
@@ -1943,7 +1940,7 @@
         <v>62</v>
       </c>
       <c r="Q16" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R16" s="32">
         <v>1</v>
@@ -1960,10 +1957,10 @@
       </c>
       <c r="V16" s="33"/>
       <c r="W16" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y16" s="5"/>
     </row>
@@ -1972,7 +1969,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>63</v>
@@ -2034,10 +2031,10 @@
       </c>
       <c r="V17" s="4"/>
       <c r="W17" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
@@ -2045,7 +2042,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>63</v>
@@ -2090,7 +2087,7 @@
         <v>10</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R18" s="32">
         <v>1</v>
@@ -2107,10 +2104,10 @@
       </c>
       <c r="V18" s="33"/>
       <c r="W18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y18" s="5"/>
     </row>
@@ -2119,7 +2116,7 @@
         <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>63</v>
@@ -2164,7 +2161,7 @@
         <v>10</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R19" s="32" t="s">
         <v>16</v>
@@ -2181,10 +2178,10 @@
       </c>
       <c r="V19" s="33"/>
       <c r="W19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X19" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Y19" s="5"/>
     </row>
@@ -2193,10 +2190,10 @@
         <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -2238,7 +2235,7 @@
         <v>10</v>
       </c>
       <c r="Q20" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R20" s="19" t="s">
         <v>16</v>
@@ -2251,14 +2248,14 @@
       </c>
       <c r="U20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1010100x001100001001x0x</v>
+        <v>0101100x001100001001x0x</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X20" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
@@ -2266,7 +2263,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>63</v>
@@ -2308,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q21" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R21" s="19">
         <v>0</v>
@@ -2328,18 +2325,18 @@
       </c>
       <c r="V21" s="4"/>
       <c r="W21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>63</v>
@@ -2381,10 +2378,10 @@
         <v>0</v>
       </c>
       <c r="P22" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q22" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R22" s="19">
         <v>0</v>
@@ -2401,10 +2398,10 @@
       </c>
       <c r="V22" s="4"/>
       <c r="W22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -2412,7 +2409,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>63</v>
@@ -2454,10 +2451,10 @@
         <v>0</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q23" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R23" s="19">
         <v>1</v>
@@ -2474,10 +2471,10 @@
       </c>
       <c r="V23" s="4"/>
       <c r="W23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -2485,7 +2482,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>63</v>
@@ -2527,10 +2524,10 @@
         <v>0</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q24" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R24" s="19">
         <v>1</v>
@@ -2547,10 +2544,10 @@
       </c>
       <c r="V24" s="4"/>
       <c r="W24" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -2558,7 +2555,7 @@
         <v>40</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>63</v>
@@ -2600,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q25" s="20" t="s">
         <v>62</v>
@@ -2620,10 +2617,10 @@
       </c>
       <c r="V25" s="4"/>
       <c r="W25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -2631,7 +2628,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>63</v>
@@ -2673,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q26" s="20" t="s">
         <v>62</v>
@@ -2693,10 +2690,10 @@
       </c>
       <c r="V26" s="4"/>
       <c r="W26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
@@ -2704,7 +2701,7 @@
         <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>63</v>
@@ -2746,10 +2743,10 @@
         <v>0</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q27" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R27" s="19" t="s">
         <v>16</v>
@@ -2766,10 +2763,10 @@
       </c>
       <c r="V27" s="4"/>
       <c r="W27" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="X27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -2777,7 +2774,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>63</v>
@@ -2822,7 +2819,7 @@
         <v>10</v>
       </c>
       <c r="Q28" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R28" s="19" t="s">
         <v>16</v>
@@ -2839,10 +2836,10 @@
       </c>
       <c r="V28" s="4"/>
       <c r="W28" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -2850,7 +2847,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>63</v>
@@ -2895,7 +2892,7 @@
         <v>62</v>
       </c>
       <c r="Q29" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R29" s="32" t="s">
         <v>16</v>
@@ -2912,10 +2909,10 @@
       </c>
       <c r="V29" s="33"/>
       <c r="W29" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X29" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Y29" s="5"/>
     </row>

</xml_diff>

<commit_message>
fix iadd control signals
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Workspaces\3rd-Year\Architecture\Pipelined-Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D25154-7232-4A70-A86F-8F9AA7BFD60D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B879098-14E2-454F-81F3-35B446380637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="134">
   <si>
     <t>operation</t>
   </si>
@@ -429,7 +429,7 @@
     <t>0000100x000110101011xx0</t>
   </si>
   <si>
-    <t>0101100x001100001001x0x</t>
+    <t>0101100x001100001001x01</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A20" sqref="A20"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2243,12 +2243,12 @@
       <c r="S20" s="4">
         <v>0</v>
       </c>
-      <c r="T20" s="19" t="s">
-        <v>16</v>
+      <c r="T20" s="19">
+        <v>1</v>
       </c>
       <c r="U20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0101100x001100001001x0x</v>
+        <v>0101100x001100001001x01</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4" t="s">

</xml_diff>

<commit_message>
fix call control signals mux1
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Workspaces\3rd-Year\Architecture\Pipelined-Processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B879098-14E2-454F-81F3-35B446380637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70543F7B-8016-4F5C-853F-32E4BB4C88FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="135">
   <si>
     <t>operation</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>0101100x001100001001x01</t>
+  </si>
+  <si>
+    <t>000001010001010000001x0</t>
   </si>
 </sst>
 </file>
@@ -788,8 +791,8 @@
   <dimension ref="A1:Y71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B20" sqref="B20"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2083,8 +2086,8 @@
       <c r="O18" s="4">
         <v>0</v>
       </c>
-      <c r="P18" s="31">
-        <v>10</v>
+      <c r="P18" s="31" t="s">
+        <v>70</v>
       </c>
       <c r="Q18" s="31" t="s">
         <v>70</v>
@@ -2100,14 +2103,14 @@
       </c>
       <c r="U18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>000001010001010010001x0</v>
+        <v>000001010001010000001x0</v>
       </c>
       <c r="V18" s="33"/>
       <c r="W18" s="4" t="s">
         <v>93</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="Y18" s="5"/>
     </row>

</xml_diff>